<commit_message>
updated excel file for print, and edited math quiz
</commit_message>
<xml_diff>
--- a/assets/various_excel_fun.xlsx
+++ b/assets/various_excel_fun.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephdecommer/Desktop/Excel Playground/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephdecommer/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9C064D-2515-4547-A473-6E49A21BB2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC327E0-A5A4-CA4B-B712-C9A09F666C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="1840" windowWidth="31740" windowHeight="21000" xr2:uid="{71485984-6B88-4A40-9EB1-AFFF2EC2C9EB}"/>
+    <workbookView xWindow="17520" yWindow="3120" windowWidth="31740" windowHeight="21000" xr2:uid="{71485984-6B88-4A40-9EB1-AFFF2EC2C9EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Functions" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Lookup Functions'!$B$2:$I$56</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -630,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A6F86B-2AAD-5F41-8A8E-110446CD62BC}">
-  <dimension ref="B2:I57"/>
+  <dimension ref="B2:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57:E57"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -644,6 +647,7 @@
     <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="24" x14ac:dyDescent="0.3">
@@ -1225,138 +1229,147 @@
         <v>809</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="24" x14ac:dyDescent="0.3">
-      <c r="B49" s="5" t="s">
+    <row r="48" spans="2:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="B48" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="3" t="s">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="H49" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I49" s="14">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="14">
+        <v>72</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" s="15">
+        <v>64901</v>
+      </c>
       <c r="H50" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I50" s="14">
+        <v>3</v>
+      </c>
+      <c r="I50" s="15">
+        <f>_xlfn.XLOOKUP(I49,C50:C56,F50:F56)</f>
+        <v>58339</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C51" s="14">
+        <v>66</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51" s="15">
+        <v>70855</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C52" s="14">
+        <v>14</v>
+      </c>
+      <c r="D52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="15">
+        <v>188657</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="14">
+        <v>30</v>
+      </c>
+      <c r="D53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" s="15">
+        <v>97566</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C54" s="14">
         <v>53</v>
       </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C51" s="14">
-        <v>72</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F51" s="15">
-        <v>64901</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I51" s="15">
-        <f>_xlfn.XLOOKUP(I50,C51:C57,F51:F57)</f>
+      <c r="D54" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" t="s">
+        <v>39</v>
+      </c>
+      <c r="F54" s="15">
         <v>58339</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C52" s="14">
-        <v>66</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F52" s="15">
-        <v>70855</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C53" s="14">
-        <v>14</v>
-      </c>
-      <c r="D53" t="s">
-        <v>32</v>
-      </c>
-      <c r="E53" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" s="15">
-        <v>188657</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="14">
-        <v>30</v>
-      </c>
-      <c r="D54" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54" s="15">
-        <v>97566</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C55" s="14">
-        <v>53</v>
-      </c>
-      <c r="D55" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" t="s">
-        <v>39</v>
+        <v>56</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F55" s="15">
-        <v>58339</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+        <v>125180</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C56" s="14">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F56" s="15">
-        <v>125180</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="14">
-        <v>79</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F57" s="15">
         <v>91632</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="60" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <rowBreaks count="2" manualBreakCount="2">
+    <brk id="1" max="16383" man="1"/>
+    <brk id="56" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="9" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
</xml_diff>